<commit_message>
Aditional MFA and PCA files
</commit_message>
<xml_diff>
--- a/Analysis/data/Motivaciones_Virgen_de_Otuzco_long.xlsx
+++ b/Analysis/data/Motivaciones_Virgen_de_Otuzco_long.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/24e4a5935cd68a2e/Documents/ESAN Papers/Otuzco/Analysis/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/24e4a5935cd68a2e/Documents/RStudioWorkspace/ESAN Proyect R/Otuzco/Analysis/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="44" documentId="8_{A19239FD-1DBD-44E3-8610-EA574720CA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{32022D1F-1323-4CA6-9EB1-680E88F882CF}"/>
+  <xr:revisionPtr revIDLastSave="48" documentId="8_{A19239FD-1DBD-44E3-8610-EA574720CA27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1D485E39-F2E4-4FE8-8F36-5C8F4C7BFC74}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{A1CFDD3B-28CA-408A-99DA-2798841D449A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{A1CFDD3B-28CA-408A-99DA-2798841D449A}"/>
   </bookViews>
   <sheets>
     <sheet name="Base de datos" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -221,6 +221,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -234,7 +240,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -286,6 +292,10 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -608,9 +618,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4058A57F-AF82-4DE8-B233-33932F02C457}">
   <dimension ref="A1:AL385"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="T9" sqref="T9"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A314" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="U322" sqref="U322"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -636,7 +646,7 @@
     <col min="19" max="19" width="50.5546875" style="18" customWidth="1"/>
     <col min="20" max="20" width="37.5546875" style="18" customWidth="1"/>
     <col min="21" max="21" width="36.88671875" style="18" customWidth="1"/>
-    <col min="22" max="22" width="39.5546875" customWidth="1"/>
+    <col min="22" max="22" width="28.44140625" style="10" customWidth="1"/>
     <col min="23" max="23" width="33.88671875" style="12" customWidth="1"/>
     <col min="24" max="24" width="31.88671875" style="12" customWidth="1"/>
     <col min="25" max="25" width="22.5546875" customWidth="1"/>
@@ -717,7 +727,7 @@
       <c r="U1" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="V1" s="24" t="s">
         <v>24</v>
       </c>
       <c r="W1" s="11" t="s">
@@ -833,7 +843,7 @@
       <c r="U2" s="18">
         <v>5</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="10">
         <v>4</v>
       </c>
       <c r="W2" s="12">
@@ -950,7 +960,7 @@
       <c r="U3" s="18">
         <v>5</v>
       </c>
-      <c r="V3">
+      <c r="V3" s="10">
         <v>2</v>
       </c>
       <c r="W3" s="12">
@@ -1066,7 +1076,7 @@
       <c r="U4" s="18">
         <v>5</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="10">
         <v>2</v>
       </c>
       <c r="W4" s="12">
@@ -1182,7 +1192,7 @@
       <c r="U5" s="18">
         <v>4</v>
       </c>
-      <c r="V5">
+      <c r="V5" s="10">
         <v>2</v>
       </c>
       <c r="W5" s="12">
@@ -1298,7 +1308,7 @@
       <c r="U6" s="18">
         <v>4</v>
       </c>
-      <c r="V6">
+      <c r="V6" s="10">
         <v>3</v>
       </c>
       <c r="W6" s="12">
@@ -1414,7 +1424,7 @@
       <c r="U7" s="18">
         <v>5</v>
       </c>
-      <c r="V7">
+      <c r="V7" s="10">
         <v>2</v>
       </c>
       <c r="W7" s="12">
@@ -1530,7 +1540,7 @@
       <c r="U8" s="18">
         <v>4</v>
       </c>
-      <c r="V8">
+      <c r="V8" s="10">
         <v>4</v>
       </c>
       <c r="W8" s="12">
@@ -1646,7 +1656,7 @@
       <c r="U9" s="18">
         <v>4</v>
       </c>
-      <c r="V9">
+      <c r="V9" s="10">
         <v>4</v>
       </c>
       <c r="W9" s="12">
@@ -1762,7 +1772,7 @@
       <c r="U10" s="18">
         <v>4</v>
       </c>
-      <c r="V10">
+      <c r="V10" s="10">
         <v>2</v>
       </c>
       <c r="W10" s="12">
@@ -1878,7 +1888,7 @@
       <c r="U11" s="18">
         <v>4</v>
       </c>
-      <c r="V11">
+      <c r="V11" s="10">
         <v>2</v>
       </c>
       <c r="W11" s="12">
@@ -1994,7 +2004,7 @@
       <c r="U12" s="18">
         <v>4</v>
       </c>
-      <c r="V12">
+      <c r="V12" s="10">
         <v>2</v>
       </c>
       <c r="W12" s="12">
@@ -2110,7 +2120,7 @@
       <c r="U13" s="18">
         <v>4</v>
       </c>
-      <c r="V13">
+      <c r="V13" s="10">
         <v>4</v>
       </c>
       <c r="W13" s="12">
@@ -2226,7 +2236,7 @@
       <c r="U14" s="18">
         <v>5</v>
       </c>
-      <c r="V14">
+      <c r="V14" s="10">
         <v>3</v>
       </c>
       <c r="W14" s="12">
@@ -2342,7 +2352,7 @@
       <c r="U15" s="18">
         <v>4</v>
       </c>
-      <c r="V15">
+      <c r="V15" s="10">
         <v>2</v>
       </c>
       <c r="W15" s="12">
@@ -2458,7 +2468,7 @@
       <c r="U16" s="18">
         <v>4</v>
       </c>
-      <c r="V16">
+      <c r="V16" s="10">
         <v>3</v>
       </c>
       <c r="W16" s="12">
@@ -2574,7 +2584,7 @@
       <c r="U17" s="18">
         <v>5</v>
       </c>
-      <c r="V17">
+      <c r="V17" s="10">
         <v>3</v>
       </c>
       <c r="W17" s="12">
@@ -2690,7 +2700,7 @@
       <c r="U18" s="18">
         <v>5</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="10">
         <v>2</v>
       </c>
       <c r="W18" s="12">
@@ -2806,7 +2816,7 @@
       <c r="U19" s="18">
         <v>4</v>
       </c>
-      <c r="V19">
+      <c r="V19" s="10">
         <v>2</v>
       </c>
       <c r="W19" s="12">
@@ -2922,7 +2932,7 @@
       <c r="U20" s="18">
         <v>5</v>
       </c>
-      <c r="V20">
+      <c r="V20" s="10">
         <v>3</v>
       </c>
       <c r="W20" s="12">
@@ -3038,7 +3048,7 @@
       <c r="U21" s="18">
         <v>5</v>
       </c>
-      <c r="V21">
+      <c r="V21" s="10">
         <v>5</v>
       </c>
       <c r="W21" s="12">
@@ -3154,7 +3164,7 @@
       <c r="U22" s="18">
         <v>4</v>
       </c>
-      <c r="V22">
+      <c r="V22" s="10">
         <v>3</v>
       </c>
       <c r="W22" s="12">
@@ -3270,7 +3280,7 @@
       <c r="U23" s="18">
         <v>4</v>
       </c>
-      <c r="V23">
+      <c r="V23" s="10">
         <v>3</v>
       </c>
       <c r="W23" s="12">
@@ -3386,7 +3396,7 @@
       <c r="U24" s="18">
         <v>5</v>
       </c>
-      <c r="V24">
+      <c r="V24" s="10">
         <v>3</v>
       </c>
       <c r="W24" s="12">
@@ -3502,7 +3512,7 @@
       <c r="U25" s="18">
         <v>5</v>
       </c>
-      <c r="V25">
+      <c r="V25" s="10">
         <v>3</v>
       </c>
       <c r="W25" s="12">
@@ -3618,7 +3628,7 @@
       <c r="U26" s="18">
         <v>5</v>
       </c>
-      <c r="V26">
+      <c r="V26" s="10">
         <v>3</v>
       </c>
       <c r="W26" s="12">
@@ -3734,7 +3744,7 @@
       <c r="U27" s="18">
         <v>5</v>
       </c>
-      <c r="V27">
+      <c r="V27" s="10">
         <v>3</v>
       </c>
       <c r="W27" s="12">
@@ -3850,7 +3860,7 @@
       <c r="U28" s="18">
         <v>5</v>
       </c>
-      <c r="V28">
+      <c r="V28" s="10">
         <v>3</v>
       </c>
       <c r="W28" s="12">
@@ -3966,7 +3976,7 @@
       <c r="U29" s="18">
         <v>5</v>
       </c>
-      <c r="V29">
+      <c r="V29" s="10">
         <v>3</v>
       </c>
       <c r="W29" s="12">
@@ -4082,7 +4092,7 @@
       <c r="U30" s="18">
         <v>5</v>
       </c>
-      <c r="V30">
+      <c r="V30" s="10">
         <v>3</v>
       </c>
       <c r="W30" s="12">
@@ -4199,7 +4209,7 @@
       <c r="U31" s="18">
         <v>5</v>
       </c>
-      <c r="V31">
+      <c r="V31" s="10">
         <v>2</v>
       </c>
       <c r="W31" s="12">
@@ -4315,7 +4325,7 @@
       <c r="U32" s="18">
         <v>5</v>
       </c>
-      <c r="V32">
+      <c r="V32" s="10">
         <v>5</v>
       </c>
       <c r="W32" s="12">
@@ -4431,7 +4441,7 @@
       <c r="U33" s="18">
         <v>5</v>
       </c>
-      <c r="V33">
+      <c r="V33" s="10">
         <v>4</v>
       </c>
       <c r="W33" s="12">
@@ -4547,7 +4557,7 @@
       <c r="U34" s="18">
         <v>5</v>
       </c>
-      <c r="V34">
+      <c r="V34" s="10">
         <v>3</v>
       </c>
       <c r="W34" s="12">
@@ -4663,7 +4673,7 @@
       <c r="U35" s="18">
         <v>5</v>
       </c>
-      <c r="V35">
+      <c r="V35" s="10">
         <v>3</v>
       </c>
       <c r="W35" s="12">
@@ -4779,7 +4789,7 @@
       <c r="U36" s="18">
         <v>5</v>
       </c>
-      <c r="V36">
+      <c r="V36" s="10">
         <v>5</v>
       </c>
       <c r="W36" s="12">
@@ -4895,7 +4905,7 @@
       <c r="U37" s="18">
         <v>5</v>
       </c>
-      <c r="V37">
+      <c r="V37" s="10">
         <v>5</v>
       </c>
       <c r="W37" s="12">
@@ -5011,7 +5021,7 @@
       <c r="U38" s="18">
         <v>5</v>
       </c>
-      <c r="V38">
+      <c r="V38" s="10">
         <v>3</v>
       </c>
       <c r="W38" s="12">
@@ -5127,7 +5137,7 @@
       <c r="U39" s="18">
         <v>4</v>
       </c>
-      <c r="V39">
+      <c r="V39" s="10">
         <v>4</v>
       </c>
       <c r="W39" s="12">
@@ -5243,7 +5253,7 @@
       <c r="U40" s="18">
         <v>4</v>
       </c>
-      <c r="V40">
+      <c r="V40" s="10">
         <v>5</v>
       </c>
       <c r="W40" s="12">
@@ -5359,7 +5369,7 @@
       <c r="U41" s="18">
         <v>4</v>
       </c>
-      <c r="V41">
+      <c r="V41" s="10">
         <v>5</v>
       </c>
       <c r="W41" s="12">
@@ -5475,7 +5485,7 @@
       <c r="U42" s="18">
         <v>4</v>
       </c>
-      <c r="V42">
+      <c r="V42" s="10">
         <v>5</v>
       </c>
       <c r="W42" s="12">
@@ -5591,7 +5601,7 @@
       <c r="U43" s="18">
         <v>5</v>
       </c>
-      <c r="V43">
+      <c r="V43" s="10">
         <v>5</v>
       </c>
       <c r="W43" s="12">
@@ -5707,7 +5717,7 @@
       <c r="U44" s="18">
         <v>5</v>
       </c>
-      <c r="V44">
+      <c r="V44" s="10">
         <v>5</v>
       </c>
       <c r="W44" s="12">
@@ -5823,7 +5833,7 @@
       <c r="U45" s="18">
         <v>5</v>
       </c>
-      <c r="V45">
+      <c r="V45" s="10">
         <v>2</v>
       </c>
       <c r="W45" s="12">
@@ -5939,7 +5949,7 @@
       <c r="U46" s="18">
         <v>4</v>
       </c>
-      <c r="V46">
+      <c r="V46" s="10">
         <v>2</v>
       </c>
       <c r="W46" s="12">
@@ -6055,7 +6065,7 @@
       <c r="U47" s="18">
         <v>4</v>
       </c>
-      <c r="V47">
+      <c r="V47" s="10">
         <v>3</v>
       </c>
       <c r="W47" s="12">
@@ -6171,7 +6181,7 @@
       <c r="U48" s="18">
         <v>5</v>
       </c>
-      <c r="V48">
+      <c r="V48" s="10">
         <v>2</v>
       </c>
       <c r="W48" s="12">
@@ -6287,7 +6297,7 @@
       <c r="U49" s="18">
         <v>5</v>
       </c>
-      <c r="V49">
+      <c r="V49" s="10">
         <v>3</v>
       </c>
       <c r="W49" s="12">
@@ -6403,7 +6413,7 @@
       <c r="U50" s="18">
         <v>4</v>
       </c>
-      <c r="V50">
+      <c r="V50" s="10">
         <v>2</v>
       </c>
       <c r="W50" s="12">
@@ -6519,7 +6529,7 @@
       <c r="U51" s="18">
         <v>5</v>
       </c>
-      <c r="V51">
+      <c r="V51" s="10">
         <v>2</v>
       </c>
       <c r="W51" s="12">
@@ -6635,7 +6645,7 @@
       <c r="U52" s="18">
         <v>4</v>
       </c>
-      <c r="V52">
+      <c r="V52" s="10">
         <v>3</v>
       </c>
       <c r="W52" s="12">
@@ -6751,7 +6761,7 @@
       <c r="U53" s="18">
         <v>4</v>
       </c>
-      <c r="V53">
+      <c r="V53" s="10">
         <v>5</v>
       </c>
       <c r="W53" s="12">
@@ -6867,7 +6877,7 @@
       <c r="U54" s="18">
         <v>5</v>
       </c>
-      <c r="V54">
+      <c r="V54" s="10">
         <v>4</v>
       </c>
       <c r="W54" s="12">
@@ -6983,7 +6993,7 @@
       <c r="U55" s="18">
         <v>5</v>
       </c>
-      <c r="V55">
+      <c r="V55" s="10">
         <v>2</v>
       </c>
       <c r="W55" s="12">
@@ -7099,7 +7109,7 @@
       <c r="U56" s="18">
         <v>4</v>
       </c>
-      <c r="V56">
+      <c r="V56" s="10">
         <v>3</v>
       </c>
       <c r="W56" s="12">
@@ -7215,7 +7225,7 @@
       <c r="U57" s="18">
         <v>4</v>
       </c>
-      <c r="V57">
+      <c r="V57" s="10">
         <v>3</v>
       </c>
       <c r="W57" s="12">
@@ -7332,7 +7342,7 @@
       <c r="U58" s="18">
         <v>5</v>
       </c>
-      <c r="V58">
+      <c r="V58" s="10">
         <v>3</v>
       </c>
       <c r="W58" s="12">
@@ -7449,7 +7459,7 @@
       <c r="U59" s="18">
         <v>5</v>
       </c>
-      <c r="V59">
+      <c r="V59" s="10">
         <v>3</v>
       </c>
       <c r="W59" s="12">
@@ -7565,7 +7575,7 @@
       <c r="U60" s="18">
         <v>5</v>
       </c>
-      <c r="V60">
+      <c r="V60" s="10">
         <v>3</v>
       </c>
       <c r="W60" s="12">
@@ -7681,7 +7691,7 @@
       <c r="U61" s="18">
         <v>4</v>
       </c>
-      <c r="V61">
+      <c r="V61" s="10">
         <v>2</v>
       </c>
       <c r="W61" s="12">
@@ -7797,7 +7807,7 @@
       <c r="U62" s="18">
         <v>5</v>
       </c>
-      <c r="V62">
+      <c r="V62" s="10">
         <v>3</v>
       </c>
       <c r="W62" s="12">
@@ -7913,7 +7923,7 @@
       <c r="U63" s="18">
         <v>5</v>
       </c>
-      <c r="V63">
+      <c r="V63" s="10">
         <v>3</v>
       </c>
       <c r="W63" s="12">
@@ -8029,7 +8039,7 @@
       <c r="U64" s="18">
         <v>4</v>
       </c>
-      <c r="V64">
+      <c r="V64" s="10">
         <v>4</v>
       </c>
       <c r="W64" s="12">
@@ -8145,7 +8155,7 @@
       <c r="U65" s="18">
         <v>4</v>
       </c>
-      <c r="V65">
+      <c r="V65" s="10">
         <v>2</v>
       </c>
       <c r="W65" s="12">
@@ -8261,7 +8271,7 @@
       <c r="U66" s="18">
         <v>4</v>
       </c>
-      <c r="V66">
+      <c r="V66" s="10">
         <v>4</v>
       </c>
       <c r="W66" s="12">
@@ -8377,7 +8387,7 @@
       <c r="U67" s="18">
         <v>5</v>
       </c>
-      <c r="V67">
+      <c r="V67" s="10">
         <v>3</v>
       </c>
       <c r="W67" s="12">
@@ -8493,7 +8503,7 @@
       <c r="U68" s="18">
         <v>4</v>
       </c>
-      <c r="V68">
+      <c r="V68" s="10">
         <v>2</v>
       </c>
       <c r="W68" s="12">
@@ -8609,7 +8619,7 @@
       <c r="U69" s="18">
         <v>4</v>
       </c>
-      <c r="V69">
+      <c r="V69" s="10">
         <v>3</v>
       </c>
       <c r="W69" s="12">
@@ -8725,7 +8735,7 @@
       <c r="U70" s="18">
         <v>5</v>
       </c>
-      <c r="V70">
+      <c r="V70" s="10">
         <v>3</v>
       </c>
       <c r="W70" s="12">
@@ -8841,7 +8851,7 @@
       <c r="U71" s="18">
         <v>5</v>
       </c>
-      <c r="V71">
+      <c r="V71" s="10">
         <v>2</v>
       </c>
       <c r="W71" s="12">
@@ -8957,7 +8967,7 @@
       <c r="U72" s="18">
         <v>4</v>
       </c>
-      <c r="V72">
+      <c r="V72" s="10">
         <v>2</v>
       </c>
       <c r="W72" s="12">
@@ -9073,7 +9083,7 @@
       <c r="U73" s="18">
         <v>5</v>
       </c>
-      <c r="V73">
+      <c r="V73" s="10">
         <v>3</v>
       </c>
       <c r="W73" s="12">
@@ -9189,7 +9199,7 @@
       <c r="U74" s="18">
         <v>4</v>
       </c>
-      <c r="V74">
+      <c r="V74" s="10">
         <v>4</v>
       </c>
       <c r="W74" s="12">
@@ -9305,7 +9315,7 @@
       <c r="U75" s="18">
         <v>4</v>
       </c>
-      <c r="V75">
+      <c r="V75" s="10">
         <v>5</v>
       </c>
       <c r="W75" s="12">
@@ -9421,7 +9431,7 @@
       <c r="U76" s="18">
         <v>4</v>
       </c>
-      <c r="V76">
+      <c r="V76" s="10">
         <v>5</v>
       </c>
       <c r="W76" s="12">
@@ -9537,7 +9547,7 @@
       <c r="U77" s="18">
         <v>4</v>
       </c>
-      <c r="V77">
+      <c r="V77" s="10">
         <v>5</v>
       </c>
       <c r="W77" s="12">
@@ -9653,7 +9663,7 @@
       <c r="U78" s="18">
         <v>5</v>
       </c>
-      <c r="V78">
+      <c r="V78" s="10">
         <v>5</v>
       </c>
       <c r="W78" s="12">
@@ -9769,7 +9779,7 @@
       <c r="U79" s="18">
         <v>5</v>
       </c>
-      <c r="V79">
+      <c r="V79" s="10">
         <v>5</v>
       </c>
       <c r="W79" s="12">
@@ -9885,7 +9895,7 @@
       <c r="U80" s="18">
         <v>5</v>
       </c>
-      <c r="V80">
+      <c r="V80" s="10">
         <v>2</v>
       </c>
       <c r="W80" s="12">
@@ -10001,7 +10011,7 @@
       <c r="U81" s="18">
         <v>4</v>
       </c>
-      <c r="V81">
+      <c r="V81" s="10">
         <v>2</v>
       </c>
       <c r="W81" s="12">
@@ -10117,7 +10127,7 @@
       <c r="U82" s="18">
         <v>4</v>
       </c>
-      <c r="V82">
+      <c r="V82" s="10">
         <v>3</v>
       </c>
       <c r="W82" s="12">
@@ -10233,7 +10243,7 @@
       <c r="U83" s="18">
         <v>5</v>
       </c>
-      <c r="V83">
+      <c r="V83" s="10">
         <v>2</v>
       </c>
       <c r="W83" s="12">
@@ -10349,7 +10359,7 @@
       <c r="U84" s="18">
         <v>5</v>
       </c>
-      <c r="V84">
+      <c r="V84" s="10">
         <v>3</v>
       </c>
       <c r="W84" s="12">
@@ -10465,7 +10475,7 @@
       <c r="U85" s="18">
         <v>4</v>
       </c>
-      <c r="V85">
+      <c r="V85" s="10">
         <v>2</v>
       </c>
       <c r="W85" s="12">
@@ -10581,7 +10591,7 @@
       <c r="U86" s="18">
         <v>5</v>
       </c>
-      <c r="V86">
+      <c r="V86" s="10">
         <v>5</v>
       </c>
       <c r="W86" s="12">
@@ -10697,7 +10707,7 @@
       <c r="U87" s="18">
         <v>5</v>
       </c>
-      <c r="V87">
+      <c r="V87" s="10">
         <v>5</v>
       </c>
       <c r="W87" s="12">
@@ -10813,7 +10823,7 @@
       <c r="U88" s="18">
         <v>5</v>
       </c>
-      <c r="V88">
+      <c r="V88" s="10">
         <v>5</v>
       </c>
       <c r="W88" s="12">
@@ -10929,7 +10939,7 @@
       <c r="U89" s="18">
         <v>5</v>
       </c>
-      <c r="V89">
+      <c r="V89" s="10">
         <v>5</v>
       </c>
       <c r="W89" s="12">
@@ -11045,7 +11055,7 @@
       <c r="U90" s="18">
         <v>5</v>
       </c>
-      <c r="V90">
+      <c r="V90" s="10">
         <v>5</v>
       </c>
       <c r="W90" s="12">
@@ -11161,7 +11171,7 @@
       <c r="U91" s="18">
         <v>5</v>
       </c>
-      <c r="V91">
+      <c r="V91" s="10">
         <v>5</v>
       </c>
       <c r="W91" s="12">
@@ -11277,7 +11287,7 @@
       <c r="U92" s="18">
         <v>4</v>
       </c>
-      <c r="V92">
+      <c r="V92" s="10">
         <v>5</v>
       </c>
       <c r="W92" s="12">
@@ -11393,7 +11403,7 @@
       <c r="U93" s="18">
         <v>5</v>
       </c>
-      <c r="V93">
+      <c r="V93" s="10">
         <v>5</v>
       </c>
       <c r="W93" s="12">
@@ -11509,7 +11519,7 @@
       <c r="U94" s="18">
         <v>5</v>
       </c>
-      <c r="V94">
+      <c r="V94" s="10">
         <v>5</v>
       </c>
       <c r="W94" s="12">
@@ -11625,7 +11635,7 @@
       <c r="U95" s="18">
         <v>5</v>
       </c>
-      <c r="V95">
+      <c r="V95" s="10">
         <v>5</v>
       </c>
       <c r="W95" s="12">
@@ -11741,7 +11751,7 @@
       <c r="U96" s="18">
         <v>5</v>
       </c>
-      <c r="V96">
+      <c r="V96" s="10">
         <v>2</v>
       </c>
       <c r="W96" s="12">
@@ -11857,7 +11867,7 @@
       <c r="U97" s="18">
         <v>4</v>
       </c>
-      <c r="V97">
+      <c r="V97" s="10">
         <v>2</v>
       </c>
       <c r="W97" s="12">
@@ -11973,7 +11983,7 @@
       <c r="U98" s="18">
         <v>4</v>
       </c>
-      <c r="V98">
+      <c r="V98" s="10">
         <v>3</v>
       </c>
       <c r="W98" s="12">
@@ -12089,7 +12099,7 @@
       <c r="U99" s="18">
         <v>5</v>
       </c>
-      <c r="V99">
+      <c r="V99" s="10">
         <v>2</v>
       </c>
       <c r="W99" s="12">
@@ -12205,7 +12215,7 @@
       <c r="U100" s="18">
         <v>4</v>
       </c>
-      <c r="V100">
+      <c r="V100" s="10">
         <v>4</v>
       </c>
       <c r="W100" s="12">
@@ -12321,7 +12331,7 @@
       <c r="U101" s="18">
         <v>4</v>
       </c>
-      <c r="V101">
+      <c r="V101" s="10">
         <v>4</v>
       </c>
       <c r="W101" s="12">
@@ -12437,7 +12447,7 @@
       <c r="U102" s="18">
         <v>4</v>
       </c>
-      <c r="V102">
+      <c r="V102" s="10">
         <v>2</v>
       </c>
       <c r="W102" s="12">
@@ -12553,7 +12563,7 @@
       <c r="U103" s="18">
         <v>4</v>
       </c>
-      <c r="V103">
+      <c r="V103" s="10">
         <v>2</v>
       </c>
       <c r="W103" s="12">
@@ -12669,7 +12679,7 @@
       <c r="U104" s="18">
         <v>4</v>
       </c>
-      <c r="V104">
+      <c r="V104" s="10">
         <v>2</v>
       </c>
       <c r="W104" s="12">
@@ -12785,7 +12795,7 @@
       <c r="U105" s="18">
         <v>4</v>
       </c>
-      <c r="V105">
+      <c r="V105" s="10">
         <v>4</v>
       </c>
       <c r="W105" s="12">
@@ -12901,7 +12911,7 @@
       <c r="U106" s="18">
         <v>5</v>
       </c>
-      <c r="V106">
+      <c r="V106" s="10">
         <v>3</v>
       </c>
       <c r="W106" s="12">
@@ -13017,7 +13027,7 @@
       <c r="U107" s="18">
         <v>4</v>
       </c>
-      <c r="V107">
+      <c r="V107" s="10">
         <v>2</v>
       </c>
       <c r="W107" s="12">
@@ -13133,7 +13143,7 @@
       <c r="U108" s="18">
         <v>4</v>
       </c>
-      <c r="V108">
+      <c r="V108" s="10">
         <v>3</v>
       </c>
       <c r="W108" s="12">
@@ -13249,7 +13259,7 @@
       <c r="U109" s="18">
         <v>5</v>
       </c>
-      <c r="V109">
+      <c r="V109" s="10">
         <v>3</v>
       </c>
       <c r="W109" s="12">
@@ -13365,7 +13375,7 @@
       <c r="U110" s="18">
         <v>5</v>
       </c>
-      <c r="V110">
+      <c r="V110" s="10">
         <v>2</v>
       </c>
       <c r="W110" s="12">
@@ -13481,7 +13491,7 @@
       <c r="U111" s="18">
         <v>5</v>
       </c>
-      <c r="V111">
+      <c r="V111" s="10">
         <v>3</v>
       </c>
       <c r="W111" s="12">
@@ -13597,7 +13607,7 @@
       <c r="U112" s="18">
         <v>5</v>
       </c>
-      <c r="V112">
+      <c r="V112" s="10">
         <v>2</v>
       </c>
       <c r="W112" s="12">
@@ -13713,7 +13723,7 @@
       <c r="U113" s="18">
         <v>5</v>
       </c>
-      <c r="V113">
+      <c r="V113" s="10">
         <v>3</v>
       </c>
       <c r="W113" s="12">
@@ -13829,7 +13839,7 @@
       <c r="U114" s="18">
         <v>4</v>
       </c>
-      <c r="V114">
+      <c r="V114" s="10">
         <v>2</v>
       </c>
       <c r="W114" s="12">
@@ -13945,7 +13955,7 @@
       <c r="U115" s="18">
         <v>3</v>
       </c>
-      <c r="V115">
+      <c r="V115" s="10">
         <v>3</v>
       </c>
       <c r="W115" s="12">
@@ -14061,7 +14071,7 @@
       <c r="U116" s="18">
         <v>4</v>
       </c>
-      <c r="V116">
+      <c r="V116" s="10">
         <v>4</v>
       </c>
       <c r="W116" s="12">
@@ -14177,7 +14187,7 @@
       <c r="U117" s="18">
         <v>5</v>
       </c>
-      <c r="V117">
+      <c r="V117" s="10">
         <v>3</v>
       </c>
       <c r="W117" s="12">
@@ -14293,7 +14303,7 @@
       <c r="U118" s="18">
         <v>5</v>
       </c>
-      <c r="V118">
+      <c r="V118" s="10">
         <v>5</v>
       </c>
       <c r="W118" s="12">
@@ -14409,7 +14419,7 @@
       <c r="U119" s="18">
         <v>5</v>
       </c>
-      <c r="V119">
+      <c r="V119" s="10">
         <v>3</v>
       </c>
       <c r="W119" s="12">
@@ -14525,7 +14535,7 @@
       <c r="U120" s="18">
         <v>5</v>
       </c>
-      <c r="V120">
+      <c r="V120" s="10">
         <v>2</v>
       </c>
       <c r="W120" s="12">
@@ -14641,7 +14651,7 @@
       <c r="U121" s="18">
         <v>4</v>
       </c>
-      <c r="V121">
+      <c r="V121" s="10">
         <v>2</v>
       </c>
       <c r="W121" s="12">
@@ -14757,7 +14767,7 @@
       <c r="U122" s="18">
         <v>5</v>
       </c>
-      <c r="V122">
+      <c r="V122" s="10">
         <v>5</v>
       </c>
       <c r="W122" s="12">
@@ -14825,6 +14835,9 @@
       <c r="E123" s="20">
         <v>5</v>
       </c>
+      <c r="F123" s="23">
+        <v>4</v>
+      </c>
       <c r="G123" s="14">
         <v>5</v>
       </c>
@@ -14870,7 +14883,7 @@
       <c r="U123" s="18">
         <v>5</v>
       </c>
-      <c r="V123">
+      <c r="V123" s="10">
         <v>4</v>
       </c>
       <c r="W123" s="12">
@@ -14987,7 +15000,7 @@
       <c r="U124" s="18">
         <v>5</v>
       </c>
-      <c r="V124">
+      <c r="V124" s="10">
         <v>3</v>
       </c>
       <c r="W124" s="12">
@@ -15104,7 +15117,7 @@
       <c r="U125" s="18">
         <v>4</v>
       </c>
-      <c r="V125">
+      <c r="V125" s="10">
         <v>4</v>
       </c>
       <c r="W125" s="12">
@@ -15220,7 +15233,7 @@
       <c r="U126" s="18">
         <v>5</v>
       </c>
-      <c r="V126">
+      <c r="V126" s="10">
         <v>3</v>
       </c>
       <c r="W126" s="12">
@@ -15336,7 +15349,7 @@
       <c r="U127" s="18">
         <v>4</v>
       </c>
-      <c r="V127">
+      <c r="V127" s="10">
         <v>2</v>
       </c>
       <c r="W127" s="12">
@@ -15452,7 +15465,7 @@
       <c r="U128" s="18">
         <v>5</v>
       </c>
-      <c r="V128">
+      <c r="V128" s="10">
         <v>2</v>
       </c>
       <c r="W128" s="12">
@@ -15568,7 +15581,7 @@
       <c r="U129" s="18">
         <v>4</v>
       </c>
-      <c r="V129">
+      <c r="V129" s="10">
         <v>3</v>
       </c>
       <c r="W129" s="12">
@@ -15684,7 +15697,7 @@
       <c r="U130" s="18">
         <v>4</v>
       </c>
-      <c r="V130">
+      <c r="V130" s="10">
         <v>3</v>
       </c>
       <c r="W130" s="12">
@@ -15800,7 +15813,7 @@
       <c r="U131" s="18">
         <v>5</v>
       </c>
-      <c r="V131">
+      <c r="V131" s="10">
         <v>5</v>
       </c>
       <c r="W131" s="12">
@@ -15916,7 +15929,7 @@
       <c r="U132" s="18">
         <v>5</v>
       </c>
-      <c r="V132">
+      <c r="V132" s="10">
         <v>1</v>
       </c>
       <c r="W132" s="12">
@@ -16032,7 +16045,7 @@
       <c r="U133" s="18">
         <v>5</v>
       </c>
-      <c r="V133">
+      <c r="V133" s="10">
         <v>3</v>
       </c>
       <c r="W133" s="12">
@@ -16148,7 +16161,7 @@
       <c r="U134" s="18">
         <v>2</v>
       </c>
-      <c r="V134">
+      <c r="V134" s="10">
         <v>3</v>
       </c>
       <c r="W134" s="12">
@@ -16264,7 +16277,7 @@
       <c r="U135" s="18">
         <v>5</v>
       </c>
-      <c r="V135">
+      <c r="V135" s="10">
         <v>5</v>
       </c>
       <c r="W135" s="12">
@@ -16380,7 +16393,7 @@
       <c r="U136" s="18">
         <v>5</v>
       </c>
-      <c r="V136">
+      <c r="V136" s="10">
         <v>2</v>
       </c>
       <c r="W136" s="12">
@@ -16496,7 +16509,7 @@
       <c r="U137" s="18">
         <v>4</v>
       </c>
-      <c r="V137">
+      <c r="V137" s="10">
         <v>2</v>
       </c>
       <c r="W137" s="12">
@@ -16612,7 +16625,7 @@
       <c r="U138" s="18">
         <v>5</v>
       </c>
-      <c r="V138">
+      <c r="V138" s="10">
         <v>3</v>
       </c>
       <c r="W138" s="12">
@@ -16728,7 +16741,7 @@
       <c r="U139" s="18">
         <v>4</v>
       </c>
-      <c r="V139">
+      <c r="V139" s="10">
         <v>2</v>
       </c>
       <c r="W139" s="12">
@@ -16844,7 +16857,7 @@
       <c r="U140" s="18">
         <v>5</v>
       </c>
-      <c r="V140">
+      <c r="V140" s="10">
         <v>3</v>
       </c>
       <c r="W140" s="12">
@@ -16960,7 +16973,7 @@
       <c r="U141" s="18">
         <v>5</v>
       </c>
-      <c r="V141">
+      <c r="V141" s="10">
         <v>5</v>
       </c>
       <c r="W141" s="12">
@@ -17076,7 +17089,7 @@
       <c r="U142" s="18">
         <v>5</v>
       </c>
-      <c r="V142">
+      <c r="V142" s="10">
         <v>3</v>
       </c>
       <c r="W142" s="12">
@@ -17192,7 +17205,7 @@
       <c r="U143" s="18">
         <v>5</v>
       </c>
-      <c r="V143">
+      <c r="V143" s="10">
         <v>3</v>
       </c>
       <c r="W143" s="12">
@@ -17308,7 +17321,7 @@
       <c r="U144" s="18">
         <v>5</v>
       </c>
-      <c r="V144">
+      <c r="V144" s="10">
         <v>2</v>
       </c>
       <c r="W144" s="12">
@@ -17424,7 +17437,7 @@
       <c r="U145" s="18">
         <v>5</v>
       </c>
-      <c r="V145">
+      <c r="V145" s="10">
         <v>3</v>
       </c>
       <c r="W145" s="12">
@@ -17540,7 +17553,7 @@
       <c r="U146" s="18">
         <v>4</v>
       </c>
-      <c r="V146">
+      <c r="V146" s="10">
         <v>3</v>
       </c>
       <c r="W146" s="12">
@@ -17656,7 +17669,7 @@
       <c r="U147" s="18">
         <v>5</v>
       </c>
-      <c r="V147">
+      <c r="V147" s="10">
         <v>2</v>
       </c>
       <c r="W147" s="12">
@@ -17772,7 +17785,7 @@
       <c r="U148" s="18">
         <v>4</v>
       </c>
-      <c r="V148">
+      <c r="V148" s="10">
         <v>2</v>
       </c>
       <c r="W148" s="12">
@@ -17888,7 +17901,7 @@
       <c r="U149" s="18">
         <v>5</v>
       </c>
-      <c r="V149">
+      <c r="V149" s="10">
         <v>2</v>
       </c>
       <c r="W149" s="12">
@@ -18004,7 +18017,7 @@
       <c r="U150" s="18">
         <v>4</v>
       </c>
-      <c r="V150">
+      <c r="V150" s="10">
         <v>2</v>
       </c>
       <c r="W150" s="12">
@@ -18120,7 +18133,7 @@
       <c r="U151" s="18">
         <v>5</v>
       </c>
-      <c r="V151">
+      <c r="V151" s="10">
         <v>5</v>
       </c>
       <c r="W151" s="12">
@@ -18236,7 +18249,7 @@
       <c r="U152" s="18">
         <v>5</v>
       </c>
-      <c r="V152">
+      <c r="V152" s="10">
         <v>3</v>
       </c>
       <c r="W152" s="12">
@@ -18352,7 +18365,7 @@
       <c r="U153" s="18">
         <v>5</v>
       </c>
-      <c r="V153">
+      <c r="V153" s="10">
         <v>3</v>
       </c>
       <c r="W153" s="12">
@@ -18468,7 +18481,7 @@
       <c r="U154" s="18">
         <v>5</v>
       </c>
-      <c r="V154">
+      <c r="V154" s="10">
         <v>3</v>
       </c>
       <c r="W154" s="12">
@@ -18584,7 +18597,7 @@
       <c r="U155" s="18">
         <v>4</v>
       </c>
-      <c r="V155">
+      <c r="V155" s="10">
         <v>3</v>
       </c>
       <c r="W155" s="12">
@@ -18700,7 +18713,7 @@
       <c r="U156" s="18">
         <v>4</v>
       </c>
-      <c r="V156">
+      <c r="V156" s="10">
         <v>3</v>
       </c>
       <c r="W156" s="12">
@@ -18816,7 +18829,7 @@
       <c r="U157" s="18">
         <v>5</v>
       </c>
-      <c r="V157">
+      <c r="V157" s="10">
         <v>5</v>
       </c>
       <c r="W157" s="12">
@@ -18932,7 +18945,7 @@
       <c r="U158" s="18">
         <v>5</v>
       </c>
-      <c r="V158">
+      <c r="V158" s="10">
         <v>1</v>
       </c>
       <c r="W158" s="12">
@@ -19048,7 +19061,7 @@
       <c r="U159" s="18">
         <v>5</v>
       </c>
-      <c r="V159">
+      <c r="V159" s="10">
         <v>3</v>
       </c>
       <c r="W159" s="12">
@@ -19164,7 +19177,7 @@
       <c r="U160" s="18">
         <v>5</v>
       </c>
-      <c r="V160">
+      <c r="V160" s="10">
         <v>2</v>
       </c>
       <c r="W160" s="12">
@@ -19280,7 +19293,7 @@
       <c r="U161" s="18">
         <v>5</v>
       </c>
-      <c r="V161">
+      <c r="V161" s="10">
         <v>3</v>
       </c>
       <c r="W161" s="12">
@@ -19396,7 +19409,7 @@
       <c r="U162" s="18">
         <v>4</v>
       </c>
-      <c r="V162">
+      <c r="V162" s="10">
         <v>3</v>
       </c>
       <c r="W162" s="12">
@@ -19512,7 +19525,7 @@
       <c r="U163" s="18">
         <v>5</v>
       </c>
-      <c r="V163">
+      <c r="V163" s="10">
         <v>5</v>
       </c>
       <c r="W163" s="12">
@@ -19628,7 +19641,7 @@
       <c r="U164" s="18">
         <v>5</v>
       </c>
-      <c r="V164">
+      <c r="V164" s="10">
         <v>5</v>
       </c>
       <c r="W164" s="12">
@@ -19744,7 +19757,7 @@
       <c r="U165" s="18">
         <v>4</v>
       </c>
-      <c r="V165">
+      <c r="V165" s="10">
         <v>5</v>
       </c>
       <c r="W165" s="12">
@@ -19860,7 +19873,7 @@
       <c r="U166" s="18">
         <v>5</v>
       </c>
-      <c r="V166">
+      <c r="V166" s="10">
         <v>4</v>
       </c>
       <c r="W166" s="12">
@@ -19976,7 +19989,7 @@
       <c r="U167" s="18">
         <v>5</v>
       </c>
-      <c r="V167">
+      <c r="V167" s="10">
         <v>5</v>
       </c>
       <c r="W167" s="12">
@@ -20092,7 +20105,7 @@
       <c r="U168" s="18">
         <v>5</v>
       </c>
-      <c r="V168">
+      <c r="V168" s="10">
         <v>5</v>
       </c>
       <c r="W168" s="12">
@@ -20208,7 +20221,7 @@
       <c r="U169" s="18">
         <v>5</v>
       </c>
-      <c r="V169">
+      <c r="V169" s="10">
         <v>5</v>
       </c>
       <c r="W169" s="12">
@@ -20325,7 +20338,7 @@
       <c r="U170" s="18">
         <v>5</v>
       </c>
-      <c r="V170">
+      <c r="V170" s="10">
         <v>3</v>
       </c>
       <c r="W170" s="12">
@@ -20442,7 +20455,7 @@
       <c r="U171" s="18">
         <v>4</v>
       </c>
-      <c r="V171">
+      <c r="V171" s="10">
         <v>4</v>
       </c>
       <c r="W171" s="12">
@@ -20558,7 +20571,7 @@
       <c r="U172" s="18">
         <v>5</v>
       </c>
-      <c r="V172">
+      <c r="V172" s="10">
         <v>3</v>
       </c>
       <c r="W172" s="12">
@@ -20674,7 +20687,7 @@
       <c r="U173" s="18">
         <v>4</v>
       </c>
-      <c r="V173">
+      <c r="V173" s="10">
         <v>2</v>
       </c>
       <c r="W173" s="12">
@@ -20790,7 +20803,7 @@
       <c r="U174" s="18">
         <v>5</v>
       </c>
-      <c r="V174">
+      <c r="V174" s="10">
         <v>2</v>
       </c>
       <c r="W174" s="12">
@@ -20906,7 +20919,7 @@
       <c r="U175" s="18">
         <v>4</v>
       </c>
-      <c r="V175">
+      <c r="V175" s="10">
         <v>3</v>
       </c>
       <c r="W175" s="12">
@@ -21023,7 +21036,7 @@
       <c r="U176" s="18">
         <v>5</v>
       </c>
-      <c r="V176">
+      <c r="V176" s="10">
         <v>3</v>
       </c>
       <c r="W176" s="12">
@@ -21140,7 +21153,7 @@
       <c r="U177" s="18">
         <v>5</v>
       </c>
-      <c r="V177">
+      <c r="V177" s="10">
         <v>4</v>
       </c>
       <c r="W177" s="12">
@@ -21256,7 +21269,7 @@
       <c r="U178" s="18">
         <v>4</v>
       </c>
-      <c r="V178">
+      <c r="V178" s="10">
         <v>4</v>
       </c>
       <c r="W178" s="12">
@@ -21372,7 +21385,7 @@
       <c r="U179" s="18">
         <v>5</v>
       </c>
-      <c r="V179">
+      <c r="V179" s="10">
         <v>2</v>
       </c>
       <c r="W179" s="12">
@@ -21488,7 +21501,7 @@
       <c r="U180" s="18">
         <v>5</v>
       </c>
-      <c r="V180">
+      <c r="V180" s="10">
         <v>3</v>
       </c>
       <c r="W180" s="12">
@@ -21604,7 +21617,7 @@
       <c r="U181" s="18">
         <v>5</v>
       </c>
-      <c r="V181">
+      <c r="V181" s="10">
         <v>3</v>
       </c>
       <c r="W181" s="12">
@@ -21720,7 +21733,7 @@
       <c r="U182" s="18">
         <v>5</v>
       </c>
-      <c r="V182">
+      <c r="V182" s="10">
         <v>2</v>
       </c>
       <c r="W182" s="12">
@@ -21836,7 +21849,7 @@
       <c r="U183" s="18">
         <v>4</v>
       </c>
-      <c r="V183">
+      <c r="V183" s="10">
         <v>3</v>
       </c>
       <c r="W183" s="12">
@@ -21952,7 +21965,7 @@
       <c r="U184" s="18">
         <v>5</v>
       </c>
-      <c r="V184">
+      <c r="V184" s="10">
         <v>2</v>
       </c>
       <c r="W184" s="12">
@@ -22068,7 +22081,7 @@
       <c r="U185" s="18">
         <v>4</v>
       </c>
-      <c r="V185">
+      <c r="V185" s="10">
         <v>3</v>
       </c>
       <c r="W185" s="12">
@@ -22184,7 +22197,7 @@
       <c r="U186" s="18">
         <v>4</v>
       </c>
-      <c r="V186">
+      <c r="V186" s="10">
         <v>2</v>
       </c>
       <c r="W186" s="12">
@@ -22300,7 +22313,7 @@
       <c r="U187" s="18">
         <v>4</v>
       </c>
-      <c r="V187">
+      <c r="V187" s="10">
         <v>3</v>
       </c>
       <c r="W187" s="12">
@@ -22416,7 +22429,7 @@
       <c r="U188" s="18">
         <v>4</v>
       </c>
-      <c r="V188">
+      <c r="V188" s="10">
         <v>1</v>
       </c>
       <c r="W188" s="12">
@@ -22532,7 +22545,7 @@
       <c r="U189" s="18">
         <v>5</v>
       </c>
-      <c r="V189">
+      <c r="V189" s="10">
         <v>1</v>
       </c>
       <c r="W189" s="12">
@@ -22648,7 +22661,7 @@
       <c r="U190" s="18">
         <v>4</v>
       </c>
-      <c r="V190">
+      <c r="V190" s="10">
         <v>3</v>
       </c>
       <c r="W190" s="12">
@@ -22764,7 +22777,7 @@
       <c r="U191" s="18">
         <v>5</v>
       </c>
-      <c r="V191">
+      <c r="V191" s="10">
         <v>2</v>
       </c>
       <c r="W191" s="12">
@@ -22880,7 +22893,7 @@
       <c r="U192" s="18">
         <v>4</v>
       </c>
-      <c r="V192">
+      <c r="V192" s="10">
         <v>3</v>
       </c>
       <c r="W192" s="12">
@@ -22996,7 +23009,7 @@
       <c r="U193" s="18">
         <v>5</v>
       </c>
-      <c r="V193">
+      <c r="V193" s="10">
         <v>5</v>
       </c>
       <c r="W193" s="12">
@@ -23112,7 +23125,7 @@
       <c r="U194" s="18">
         <v>5</v>
       </c>
-      <c r="V194">
+      <c r="V194" s="10">
         <v>2</v>
       </c>
       <c r="W194" s="12">
@@ -23228,7 +23241,7 @@
       <c r="U195" s="18">
         <v>5</v>
       </c>
-      <c r="V195">
+      <c r="V195" s="10">
         <v>5</v>
       </c>
       <c r="W195" s="12">
@@ -23344,7 +23357,7 @@
       <c r="U196" s="18">
         <v>5</v>
       </c>
-      <c r="V196">
+      <c r="V196" s="10">
         <v>5</v>
       </c>
       <c r="W196" s="12">
@@ -23460,7 +23473,7 @@
       <c r="U197" s="18">
         <v>5</v>
       </c>
-      <c r="V197">
+      <c r="V197" s="10">
         <v>5</v>
       </c>
       <c r="W197" s="12">
@@ -23576,7 +23589,7 @@
       <c r="U198" s="18">
         <v>5</v>
       </c>
-      <c r="V198">
+      <c r="V198" s="10">
         <v>5</v>
       </c>
       <c r="W198" s="12">
@@ -23692,7 +23705,7 @@
       <c r="U199" s="18">
         <v>4</v>
       </c>
-      <c r="V199">
+      <c r="V199" s="10">
         <v>4</v>
       </c>
       <c r="W199" s="12">
@@ -23808,7 +23821,7 @@
       <c r="U200" s="18">
         <v>5</v>
       </c>
-      <c r="V200">
+      <c r="V200" s="10">
         <v>2</v>
       </c>
       <c r="W200" s="12">
@@ -23924,7 +23937,7 @@
       <c r="U201" s="18">
         <v>5</v>
       </c>
-      <c r="V201">
+      <c r="V201" s="10">
         <v>4</v>
       </c>
       <c r="W201" s="12">
@@ -24040,7 +24053,7 @@
       <c r="U202" s="18">
         <v>4</v>
       </c>
-      <c r="V202">
+      <c r="V202" s="10">
         <v>2</v>
       </c>
       <c r="W202" s="12">
@@ -24156,7 +24169,7 @@
       <c r="U203" s="18">
         <v>4</v>
       </c>
-      <c r="V203">
+      <c r="V203" s="10">
         <v>3</v>
       </c>
       <c r="W203" s="12">
@@ -24272,7 +24285,7 @@
       <c r="U204" s="18">
         <v>5</v>
       </c>
-      <c r="V204">
+      <c r="V204" s="10">
         <v>3</v>
       </c>
       <c r="W204" s="12">
@@ -24388,7 +24401,7 @@
       <c r="U205" s="18">
         <v>5</v>
       </c>
-      <c r="V205">
+      <c r="V205" s="10">
         <v>2</v>
       </c>
       <c r="W205" s="12">
@@ -24504,7 +24517,7 @@
       <c r="U206" s="18">
         <v>5</v>
       </c>
-      <c r="V206">
+      <c r="V206" s="10">
         <v>2</v>
       </c>
       <c r="W206" s="12">
@@ -24621,7 +24634,7 @@
       <c r="U207" s="18">
         <v>5</v>
       </c>
-      <c r="V207">
+      <c r="V207" s="10">
         <v>2</v>
       </c>
       <c r="W207" s="12">
@@ -24738,7 +24751,7 @@
       <c r="U208" s="18">
         <v>5</v>
       </c>
-      <c r="V208">
+      <c r="V208" s="10">
         <v>2</v>
       </c>
       <c r="W208" s="12">
@@ -24855,7 +24868,7 @@
       <c r="U209" s="18">
         <v>5</v>
       </c>
-      <c r="V209">
+      <c r="V209" s="10">
         <v>4</v>
       </c>
       <c r="W209" s="12">
@@ -24971,7 +24984,7 @@
       <c r="U210" s="18">
         <v>5</v>
       </c>
-      <c r="V210">
+      <c r="V210" s="10">
         <v>4</v>
       </c>
       <c r="W210" s="12">
@@ -25087,7 +25100,7 @@
       <c r="U211" s="18">
         <v>4</v>
       </c>
-      <c r="V211">
+      <c r="V211" s="10">
         <v>4</v>
       </c>
       <c r="W211" s="12">
@@ -25203,7 +25216,7 @@
       <c r="U212" s="18">
         <v>4</v>
       </c>
-      <c r="V212">
+      <c r="V212" s="10">
         <v>3</v>
       </c>
       <c r="W212" s="12">
@@ -25319,7 +25332,7 @@
       <c r="U213" s="18">
         <v>5</v>
       </c>
-      <c r="V213">
+      <c r="V213" s="10">
         <v>2</v>
       </c>
       <c r="W213" s="12">
@@ -25435,7 +25448,7 @@
       <c r="U214" s="18">
         <v>5</v>
       </c>
-      <c r="V214">
+      <c r="V214" s="10">
         <v>2</v>
       </c>
       <c r="W214" s="12">
@@ -25551,7 +25564,7 @@
       <c r="U215" s="18">
         <v>4</v>
       </c>
-      <c r="V215">
+      <c r="V215" s="10">
         <v>3</v>
       </c>
       <c r="W215" s="12">
@@ -25667,7 +25680,7 @@
       <c r="U216" s="18">
         <v>4</v>
       </c>
-      <c r="V216">
+      <c r="V216" s="10">
         <v>4</v>
       </c>
       <c r="W216" s="12">
@@ -25783,7 +25796,7 @@
       <c r="U217" s="18">
         <v>5</v>
       </c>
-      <c r="V217">
+      <c r="V217" s="10">
         <v>3</v>
       </c>
       <c r="W217" s="12">
@@ -25899,7 +25912,7 @@
       <c r="U218" s="18">
         <v>4</v>
       </c>
-      <c r="V218">
+      <c r="V218" s="10">
         <v>2</v>
       </c>
       <c r="W218" s="12">
@@ -26015,7 +26028,7 @@
       <c r="U219" s="18">
         <v>5</v>
       </c>
-      <c r="V219">
+      <c r="V219" s="10">
         <v>2</v>
       </c>
       <c r="W219" s="12">
@@ -26131,7 +26144,7 @@
       <c r="U220" s="18">
         <v>4</v>
       </c>
-      <c r="V220">
+      <c r="V220" s="10">
         <v>5</v>
       </c>
       <c r="W220" s="12">
@@ -26247,7 +26260,7 @@
       <c r="U221" s="18">
         <v>5</v>
       </c>
-      <c r="V221">
+      <c r="V221" s="10">
         <v>2</v>
       </c>
       <c r="W221" s="12">
@@ -26363,7 +26376,7 @@
       <c r="U222" s="18">
         <v>4</v>
       </c>
-      <c r="V222">
+      <c r="V222" s="10">
         <v>5</v>
       </c>
       <c r="W222" s="12">
@@ -26479,7 +26492,7 @@
       <c r="U223" s="18">
         <v>5</v>
       </c>
-      <c r="V223">
+      <c r="V223" s="10">
         <v>3</v>
       </c>
       <c r="W223" s="12">
@@ -26596,7 +26609,7 @@
       <c r="U224" s="18">
         <v>5</v>
       </c>
-      <c r="V224">
+      <c r="V224" s="10">
         <v>2</v>
       </c>
       <c r="W224" s="12">
@@ -26712,7 +26725,7 @@
       <c r="U225" s="18">
         <v>4</v>
       </c>
-      <c r="V225">
+      <c r="V225" s="10">
         <v>4</v>
       </c>
       <c r="W225" s="12">
@@ -26828,7 +26841,7 @@
       <c r="U226" s="18">
         <v>5</v>
       </c>
-      <c r="V226">
+      <c r="V226" s="10">
         <v>3</v>
       </c>
       <c r="W226" s="12">
@@ -26944,7 +26957,7 @@
       <c r="U227" s="18">
         <v>5</v>
       </c>
-      <c r="V227">
+      <c r="V227" s="10">
         <v>2</v>
       </c>
       <c r="W227" s="12">
@@ -27060,7 +27073,7 @@
       <c r="U228" s="18">
         <v>4</v>
       </c>
-      <c r="V228">
+      <c r="V228" s="10">
         <v>3</v>
       </c>
       <c r="W228" s="12">
@@ -27176,7 +27189,7 @@
       <c r="U229" s="18">
         <v>5</v>
       </c>
-      <c r="V229">
+      <c r="V229" s="10">
         <v>2</v>
       </c>
       <c r="W229" s="12">
@@ -27292,7 +27305,7 @@
       <c r="U230" s="18">
         <v>4</v>
       </c>
-      <c r="V230">
+      <c r="V230" s="10">
         <v>3</v>
       </c>
       <c r="W230" s="12">
@@ -27408,7 +27421,7 @@
       <c r="U231" s="18">
         <v>4</v>
       </c>
-      <c r="V231">
+      <c r="V231" s="10">
         <v>2</v>
       </c>
       <c r="W231" s="12">
@@ -27524,7 +27537,7 @@
       <c r="U232" s="18">
         <v>4</v>
       </c>
-      <c r="V232">
+      <c r="V232" s="10">
         <v>3</v>
       </c>
       <c r="W232" s="12">
@@ -27640,7 +27653,7 @@
       <c r="U233" s="18">
         <v>4</v>
       </c>
-      <c r="V233">
+      <c r="V233" s="10">
         <v>1</v>
       </c>
       <c r="W233" s="12">
@@ -27756,7 +27769,7 @@
       <c r="U234" s="18">
         <v>5</v>
       </c>
-      <c r="V234">
+      <c r="V234" s="10">
         <v>1</v>
       </c>
       <c r="W234" s="12">
@@ -27872,7 +27885,7 @@
       <c r="U235" s="18">
         <v>4</v>
       </c>
-      <c r="V235">
+      <c r="V235" s="10">
         <v>3</v>
       </c>
       <c r="W235" s="12">
@@ -27988,7 +28001,7 @@
       <c r="U236" s="18">
         <v>5</v>
       </c>
-      <c r="V236">
+      <c r="V236" s="10">
         <v>2</v>
       </c>
       <c r="W236" s="12">
@@ -28104,7 +28117,7 @@
       <c r="U237" s="18">
         <v>4</v>
       </c>
-      <c r="V237">
+      <c r="V237" s="10">
         <v>3</v>
       </c>
       <c r="W237" s="12">
@@ -28220,7 +28233,7 @@
       <c r="U238" s="18">
         <v>4</v>
       </c>
-      <c r="V238">
+      <c r="V238" s="10">
         <v>4</v>
       </c>
       <c r="W238" s="12">
@@ -28336,7 +28349,7 @@
       <c r="U239" s="18">
         <v>4</v>
       </c>
-      <c r="V239">
+      <c r="V239" s="10">
         <v>3</v>
       </c>
       <c r="W239" s="12">
@@ -28452,7 +28465,7 @@
       <c r="U240" s="18">
         <v>5</v>
       </c>
-      <c r="V240">
+      <c r="V240" s="10">
         <v>2</v>
       </c>
       <c r="W240" s="12">
@@ -28568,7 +28581,7 @@
       <c r="U241" s="18">
         <v>5</v>
       </c>
-      <c r="V241">
+      <c r="V241" s="10">
         <v>2</v>
       </c>
       <c r="W241" s="12">
@@ -28684,7 +28697,7 @@
       <c r="U242" s="18">
         <v>4</v>
       </c>
-      <c r="V242">
+      <c r="V242" s="10">
         <v>3</v>
       </c>
       <c r="W242" s="12">
@@ -28800,7 +28813,7 @@
       <c r="U243" s="18">
         <v>4</v>
       </c>
-      <c r="V243">
+      <c r="V243" s="10">
         <v>4</v>
       </c>
       <c r="W243" s="12">
@@ -28916,7 +28929,7 @@
       <c r="U244" s="18">
         <v>5</v>
       </c>
-      <c r="V244">
+      <c r="V244" s="10">
         <v>3</v>
       </c>
       <c r="W244" s="12">
@@ -29032,7 +29045,7 @@
       <c r="U245" s="18">
         <v>5</v>
       </c>
-      <c r="V245">
+      <c r="V245" s="10">
         <v>5</v>
       </c>
       <c r="W245" s="12">
@@ -29148,7 +29161,7 @@
       <c r="U246" s="18">
         <v>5</v>
       </c>
-      <c r="V246">
+      <c r="V246" s="10">
         <v>5</v>
       </c>
       <c r="W246" s="12">
@@ -29264,7 +29277,7 @@
       <c r="U247" s="18">
         <v>5</v>
       </c>
-      <c r="V247">
+      <c r="V247" s="10">
         <v>5</v>
       </c>
       <c r="W247" s="12">
@@ -29380,7 +29393,7 @@
       <c r="U248" s="18">
         <v>5</v>
       </c>
-      <c r="V248">
+      <c r="V248" s="10">
         <v>5</v>
       </c>
       <c r="W248" s="12">
@@ -29496,7 +29509,7 @@
       <c r="U249" s="18">
         <v>5</v>
       </c>
-      <c r="V249">
+      <c r="V249" s="10">
         <v>3</v>
       </c>
       <c r="W249" s="12">
@@ -29612,7 +29625,7 @@
       <c r="U250" s="18">
         <v>4</v>
       </c>
-      <c r="V250">
+      <c r="V250" s="10">
         <v>4</v>
       </c>
       <c r="W250" s="12">
@@ -29728,7 +29741,7 @@
       <c r="U251" s="18">
         <v>5</v>
       </c>
-      <c r="V251">
+      <c r="V251" s="10">
         <v>5</v>
       </c>
       <c r="W251" s="12">
@@ -29844,7 +29857,7 @@
       <c r="U252" s="18">
         <v>5</v>
       </c>
-      <c r="V252">
+      <c r="V252" s="10">
         <v>4</v>
       </c>
       <c r="W252" s="12">
@@ -29960,7 +29973,7 @@
       <c r="U253" s="18">
         <v>4</v>
       </c>
-      <c r="V253">
+      <c r="V253" s="10">
         <v>4</v>
       </c>
       <c r="W253" s="12">
@@ -30076,7 +30089,7 @@
       <c r="U254" s="18">
         <v>5</v>
       </c>
-      <c r="V254">
+      <c r="V254" s="10">
         <v>2</v>
       </c>
       <c r="W254" s="12">
@@ -30192,7 +30205,7 @@
       <c r="U255" s="18">
         <v>5</v>
       </c>
-      <c r="V255">
+      <c r="V255" s="10">
         <v>3</v>
       </c>
       <c r="W255" s="12">
@@ -30308,7 +30321,7 @@
       <c r="U256" s="18">
         <v>5</v>
       </c>
-      <c r="V256">
+      <c r="V256" s="10">
         <v>3</v>
       </c>
       <c r="W256" s="12">
@@ -30424,7 +30437,7 @@
       <c r="U257" s="18">
         <v>5</v>
       </c>
-      <c r="V257">
+      <c r="V257" s="10">
         <v>2</v>
       </c>
       <c r="W257" s="12">
@@ -30540,7 +30553,7 @@
       <c r="U258" s="18">
         <v>4</v>
       </c>
-      <c r="V258">
+      <c r="V258" s="10">
         <v>3</v>
       </c>
       <c r="W258" s="12">
@@ -30656,7 +30669,7 @@
       <c r="U259" s="18">
         <v>5</v>
       </c>
-      <c r="V259">
+      <c r="V259" s="10">
         <v>2</v>
       </c>
       <c r="W259" s="12">
@@ -30772,7 +30785,7 @@
       <c r="U260" s="18">
         <v>4</v>
       </c>
-      <c r="V260">
+      <c r="V260" s="10">
         <v>3</v>
       </c>
       <c r="W260" s="12">
@@ -30885,7 +30898,7 @@
       <c r="U261" s="18">
         <v>4</v>
       </c>
-      <c r="V261">
+      <c r="V261" s="10">
         <v>2</v>
       </c>
       <c r="W261" s="12">
@@ -31001,7 +31014,7 @@
       <c r="U262" s="18">
         <v>5</v>
       </c>
-      <c r="V262">
+      <c r="V262" s="10">
         <v>3</v>
       </c>
       <c r="W262" s="12">
@@ -31117,7 +31130,7 @@
       <c r="U263" s="18">
         <v>4</v>
       </c>
-      <c r="V263">
+      <c r="V263" s="10">
         <v>2</v>
       </c>
       <c r="W263" s="12">
@@ -31233,7 +31246,7 @@
       <c r="U264" s="18">
         <v>5</v>
       </c>
-      <c r="V264">
+      <c r="V264" s="10">
         <v>3</v>
       </c>
       <c r="W264" s="12">
@@ -31349,7 +31362,7 @@
       <c r="U265" s="18">
         <v>5</v>
       </c>
-      <c r="V265">
+      <c r="V265" s="10">
         <v>4</v>
       </c>
       <c r="W265" s="12">
@@ -31465,7 +31478,7 @@
       <c r="U266" s="18">
         <v>4</v>
       </c>
-      <c r="V266">
+      <c r="V266" s="10">
         <v>3</v>
       </c>
       <c r="W266" s="12">
@@ -31581,7 +31594,7 @@
       <c r="U267" s="18">
         <v>5</v>
       </c>
-      <c r="V267">
+      <c r="V267" s="10">
         <v>3</v>
       </c>
       <c r="W267" s="12">
@@ -31697,7 +31710,7 @@
       <c r="U268" s="18">
         <v>4</v>
       </c>
-      <c r="V268">
+      <c r="V268" s="10">
         <v>3</v>
       </c>
       <c r="W268" s="12">
@@ -31813,7 +31826,7 @@
       <c r="U269" s="18">
         <v>5</v>
       </c>
-      <c r="V269">
+      <c r="V269" s="10">
         <v>3</v>
       </c>
       <c r="W269" s="12">
@@ -31929,7 +31942,7 @@
       <c r="U270" s="18">
         <v>4</v>
       </c>
-      <c r="V270">
+      <c r="V270" s="10">
         <v>2</v>
       </c>
       <c r="W270" s="12">
@@ -32045,7 +32058,7 @@
       <c r="U271" s="18">
         <v>2</v>
       </c>
-      <c r="V271">
+      <c r="V271" s="10">
         <v>5</v>
       </c>
       <c r="W271" s="12">
@@ -32161,7 +32174,7 @@
       <c r="U272" s="18">
         <v>5</v>
       </c>
-      <c r="V272">
+      <c r="V272" s="10">
         <v>4</v>
       </c>
       <c r="W272" s="12">
@@ -32277,7 +32290,7 @@
       <c r="U273" s="18">
         <v>5</v>
       </c>
-      <c r="V273">
+      <c r="V273" s="10">
         <v>4</v>
       </c>
       <c r="W273" s="12">
@@ -32393,7 +32406,7 @@
       <c r="U274" s="18">
         <v>4</v>
       </c>
-      <c r="V274">
+      <c r="V274" s="10">
         <v>2</v>
       </c>
       <c r="W274" s="12">
@@ -32509,7 +32522,7 @@
       <c r="U275" s="18">
         <v>5</v>
       </c>
-      <c r="V275">
+      <c r="V275" s="10">
         <v>2</v>
       </c>
       <c r="W275" s="12">
@@ -32625,7 +32638,7 @@
       <c r="U276" s="18">
         <v>5</v>
       </c>
-      <c r="V276">
+      <c r="V276" s="10">
         <v>5</v>
       </c>
       <c r="W276" s="12">
@@ -32741,7 +32754,7 @@
       <c r="U277" s="18">
         <v>4</v>
       </c>
-      <c r="V277">
+      <c r="V277" s="10">
         <v>3</v>
       </c>
       <c r="W277" s="12">
@@ -32857,7 +32870,7 @@
       <c r="U278" s="18">
         <v>5</v>
       </c>
-      <c r="V278">
+      <c r="V278" s="10">
         <v>3</v>
       </c>
       <c r="W278" s="12">
@@ -32973,7 +32986,7 @@
       <c r="U279" s="18">
         <v>5</v>
       </c>
-      <c r="V279">
+      <c r="V279" s="10">
         <v>4</v>
       </c>
       <c r="W279" s="12">
@@ -33089,7 +33102,7 @@
       <c r="U280" s="18">
         <v>4</v>
       </c>
-      <c r="V280">
+      <c r="V280" s="10">
         <v>4</v>
       </c>
       <c r="W280" s="12">
@@ -33205,7 +33218,7 @@
       <c r="U281" s="18">
         <v>5</v>
       </c>
-      <c r="V281">
+      <c r="V281" s="10">
         <v>3</v>
       </c>
       <c r="W281" s="12">
@@ -33321,7 +33334,7 @@
       <c r="U282" s="18">
         <v>5</v>
       </c>
-      <c r="V282">
+      <c r="V282" s="10">
         <v>4</v>
       </c>
       <c r="W282" s="12">
@@ -33437,7 +33450,7 @@
       <c r="U283" s="18">
         <v>4</v>
       </c>
-      <c r="V283">
+      <c r="V283" s="10">
         <v>4</v>
       </c>
       <c r="W283" s="12">
@@ -33553,7 +33566,7 @@
       <c r="U284" s="18">
         <v>5</v>
       </c>
-      <c r="V284">
+      <c r="V284" s="10">
         <v>2</v>
       </c>
       <c r="W284" s="12">
@@ -33670,7 +33683,7 @@
       <c r="U285" s="18">
         <v>5</v>
       </c>
-      <c r="V285">
+      <c r="V285" s="10">
         <v>2</v>
       </c>
       <c r="W285" s="12">
@@ -33786,7 +33799,7 @@
       <c r="U286" s="18">
         <v>5</v>
       </c>
-      <c r="V286">
+      <c r="V286" s="10">
         <v>2</v>
       </c>
       <c r="W286" s="12">
@@ -33902,7 +33915,7 @@
       <c r="U287" s="18">
         <v>5</v>
       </c>
-      <c r="V287">
+      <c r="V287" s="10">
         <v>2</v>
       </c>
       <c r="W287" s="12">
@@ -34018,7 +34031,7 @@
       <c r="U288" s="18">
         <v>5</v>
       </c>
-      <c r="V288">
+      <c r="V288" s="10">
         <v>4</v>
       </c>
       <c r="W288" s="12">
@@ -34134,7 +34147,7 @@
       <c r="U289" s="18">
         <v>4</v>
       </c>
-      <c r="V289">
+      <c r="V289" s="10">
         <v>4</v>
       </c>
       <c r="W289" s="12">
@@ -34250,7 +34263,7 @@
       <c r="U290" s="18">
         <v>5</v>
       </c>
-      <c r="V290">
+      <c r="V290" s="10">
         <v>3</v>
       </c>
       <c r="W290" s="12">
@@ -34366,7 +34379,7 @@
       <c r="U291" s="18">
         <v>5</v>
       </c>
-      <c r="V291">
+      <c r="V291" s="10">
         <v>2</v>
       </c>
       <c r="W291" s="12">
@@ -34482,7 +34495,7 @@
       <c r="U292" s="18">
         <v>5</v>
       </c>
-      <c r="V292">
+      <c r="V292" s="10">
         <v>3</v>
       </c>
       <c r="W292" s="12">
@@ -34598,7 +34611,7 @@
       <c r="U293" s="18">
         <v>5</v>
       </c>
-      <c r="V293">
+      <c r="V293" s="10">
         <v>2</v>
       </c>
       <c r="W293" s="12">
@@ -34714,7 +34727,7 @@
       <c r="U294" s="18">
         <v>5</v>
       </c>
-      <c r="V294">
+      <c r="V294" s="10">
         <v>3</v>
       </c>
       <c r="W294" s="12">
@@ -34830,7 +34843,7 @@
       <c r="U295" s="18">
         <v>4</v>
       </c>
-      <c r="V295">
+      <c r="V295" s="10">
         <v>2</v>
       </c>
       <c r="W295" s="12">
@@ -34946,7 +34959,7 @@
       <c r="U296" s="18">
         <v>4</v>
       </c>
-      <c r="V296">
+      <c r="V296" s="10">
         <v>2</v>
       </c>
       <c r="W296" s="12">
@@ -35062,7 +35075,7 @@
       <c r="U297" s="18">
         <v>5</v>
       </c>
-      <c r="V297">
+      <c r="V297" s="10">
         <v>3</v>
       </c>
       <c r="W297" s="12">
@@ -35178,7 +35191,7 @@
       <c r="U298" s="18">
         <v>5</v>
       </c>
-      <c r="V298">
+      <c r="V298" s="10">
         <v>4</v>
       </c>
       <c r="W298" s="12">
@@ -35294,7 +35307,7 @@
       <c r="U299" s="18">
         <v>4</v>
       </c>
-      <c r="V299">
+      <c r="V299" s="10">
         <v>3</v>
       </c>
       <c r="W299" s="12">
@@ -35410,7 +35423,7 @@
       <c r="U300" s="18">
         <v>5</v>
       </c>
-      <c r="V300">
+      <c r="V300" s="10">
         <v>3</v>
       </c>
       <c r="W300" s="12">
@@ -35526,7 +35539,7 @@
       <c r="U301" s="18">
         <v>4</v>
       </c>
-      <c r="V301">
+      <c r="V301" s="10">
         <v>3</v>
       </c>
       <c r="W301" s="12">
@@ -35642,7 +35655,7 @@
       <c r="U302" s="18">
         <v>5</v>
       </c>
-      <c r="V302">
+      <c r="V302" s="10">
         <v>3</v>
       </c>
       <c r="W302" s="12">
@@ -35758,7 +35771,7 @@
       <c r="U303" s="18">
         <v>4</v>
       </c>
-      <c r="V303">
+      <c r="V303" s="10">
         <v>2</v>
       </c>
       <c r="W303" s="12">
@@ -35874,7 +35887,7 @@
       <c r="U304" s="18">
         <v>5</v>
       </c>
-      <c r="V304">
+      <c r="V304" s="10">
         <v>2</v>
       </c>
       <c r="W304" s="12">
@@ -35990,7 +36003,7 @@
       <c r="U305" s="18">
         <v>5</v>
       </c>
-      <c r="V305">
+      <c r="V305" s="10">
         <v>4</v>
       </c>
       <c r="W305" s="12">
@@ -36106,7 +36119,7 @@
       <c r="U306" s="18">
         <v>4</v>
       </c>
-      <c r="V306">
+      <c r="V306" s="10">
         <v>4</v>
       </c>
       <c r="W306" s="12">
@@ -36222,7 +36235,7 @@
       <c r="U307" s="18">
         <v>5</v>
       </c>
-      <c r="V307">
+      <c r="V307" s="10">
         <v>3</v>
       </c>
       <c r="W307" s="12">
@@ -36338,7 +36351,7 @@
       <c r="U308" s="18">
         <v>5</v>
       </c>
-      <c r="V308">
+      <c r="V308" s="10">
         <v>2</v>
       </c>
       <c r="W308" s="12">
@@ -36454,7 +36467,7 @@
       <c r="U309" s="18">
         <v>5</v>
       </c>
-      <c r="V309">
+      <c r="V309" s="10">
         <v>3</v>
       </c>
       <c r="W309" s="12">
@@ -36570,7 +36583,7 @@
       <c r="U310" s="18">
         <v>5</v>
       </c>
-      <c r="V310">
+      <c r="V310" s="10">
         <v>2</v>
       </c>
       <c r="W310" s="12">
@@ -36686,7 +36699,7 @@
       <c r="U311" s="18">
         <v>5</v>
       </c>
-      <c r="V311">
+      <c r="V311" s="10">
         <v>3</v>
       </c>
       <c r="W311" s="12">
@@ -36802,7 +36815,7 @@
       <c r="U312" s="18">
         <v>4</v>
       </c>
-      <c r="V312">
+      <c r="V312" s="10">
         <v>2</v>
       </c>
       <c r="W312" s="12">
@@ -36918,7 +36931,7 @@
       <c r="U313" s="18">
         <v>5</v>
       </c>
-      <c r="V313">
+      <c r="V313" s="10">
         <v>5</v>
       </c>
       <c r="W313" s="12">
@@ -37034,7 +37047,7 @@
       <c r="U314" s="18">
         <v>5</v>
       </c>
-      <c r="V314">
+      <c r="V314" s="10">
         <v>4</v>
       </c>
       <c r="W314" s="12">
@@ -37150,7 +37163,7 @@
       <c r="U315" s="18">
         <v>5</v>
       </c>
-      <c r="V315">
+      <c r="V315" s="10">
         <v>4</v>
       </c>
       <c r="W315" s="12">
@@ -37266,7 +37279,7 @@
       <c r="U316" s="18">
         <v>5</v>
       </c>
-      <c r="V316">
+      <c r="V316" s="10">
         <v>5</v>
       </c>
       <c r="W316" s="12">
@@ -37382,7 +37395,7 @@
       <c r="U317" s="18">
         <v>5</v>
       </c>
-      <c r="V317">
+      <c r="V317" s="10">
         <v>5</v>
       </c>
       <c r="W317" s="12">
@@ -37498,7 +37511,7 @@
       <c r="U318" s="18">
         <v>5</v>
       </c>
-      <c r="V318">
+      <c r="V318" s="10">
         <v>3</v>
       </c>
       <c r="W318" s="12">
@@ -37614,7 +37627,7 @@
       <c r="U319" s="18">
         <v>5</v>
       </c>
-      <c r="V319">
+      <c r="V319" s="10">
         <v>4</v>
       </c>
       <c r="W319" s="12">
@@ -37730,7 +37743,7 @@
       <c r="U320" s="18">
         <v>5</v>
       </c>
-      <c r="V320">
+      <c r="V320" s="10">
         <v>5</v>
       </c>
       <c r="W320" s="12">
@@ -37846,7 +37859,7 @@
       <c r="U321" s="18">
         <v>5</v>
       </c>
-      <c r="V321">
+      <c r="V321" s="10">
         <v>5</v>
       </c>
       <c r="W321" s="12">
@@ -37962,7 +37975,7 @@
       <c r="U322" s="18">
         <v>5</v>
       </c>
-      <c r="V322">
+      <c r="V322" s="10">
         <v>5</v>
       </c>
       <c r="W322" s="12">
@@ -38078,7 +38091,7 @@
       <c r="U323" s="18">
         <v>5</v>
       </c>
-      <c r="V323">
+      <c r="V323" s="10">
         <v>5</v>
       </c>
       <c r="W323" s="12">
@@ -38194,7 +38207,7 @@
       <c r="U324" s="18">
         <v>5</v>
       </c>
-      <c r="V324">
+      <c r="V324" s="10">
         <v>5</v>
       </c>
       <c r="W324" s="12">
@@ -38310,7 +38323,7 @@
       <c r="U325" s="18">
         <v>5</v>
       </c>
-      <c r="V325">
+      <c r="V325" s="10">
         <v>5</v>
       </c>
       <c r="W325" s="12">
@@ -38426,7 +38439,7 @@
       <c r="U326" s="18">
         <v>5</v>
       </c>
-      <c r="V326">
+      <c r="V326" s="10">
         <v>3</v>
       </c>
       <c r="W326" s="12">
@@ -38542,7 +38555,7 @@
       <c r="U327" s="18">
         <v>4</v>
       </c>
-      <c r="V327">
+      <c r="V327" s="10">
         <v>2</v>
       </c>
       <c r="W327" s="12">
@@ -38658,7 +38671,7 @@
       <c r="U328" s="18">
         <v>5</v>
       </c>
-      <c r="V328">
+      <c r="V328" s="10">
         <v>3</v>
       </c>
       <c r="W328" s="12">
@@ -38774,7 +38787,7 @@
       <c r="U329" s="18">
         <v>5</v>
       </c>
-      <c r="V329">
+      <c r="V329" s="10">
         <v>4</v>
       </c>
       <c r="W329" s="12">
@@ -38890,7 +38903,7 @@
       <c r="U330" s="18">
         <v>4</v>
       </c>
-      <c r="V330">
+      <c r="V330" s="10">
         <v>3</v>
       </c>
       <c r="W330" s="12">
@@ -39006,7 +39019,7 @@
       <c r="U331" s="18">
         <v>5</v>
       </c>
-      <c r="V331">
+      <c r="V331" s="10">
         <v>3</v>
       </c>
       <c r="W331" s="12">
@@ -39122,7 +39135,7 @@
       <c r="U332" s="18">
         <v>4</v>
       </c>
-      <c r="V332">
+      <c r="V332" s="10">
         <v>2</v>
       </c>
       <c r="W332" s="12">
@@ -39238,7 +39251,7 @@
       <c r="U333" s="18">
         <v>5</v>
       </c>
-      <c r="V333">
+      <c r="V333" s="10">
         <v>3</v>
       </c>
       <c r="W333" s="12">
@@ -39354,7 +39367,7 @@
       <c r="U334" s="18">
         <v>5</v>
       </c>
-      <c r="V334">
+      <c r="V334" s="10">
         <v>5</v>
       </c>
       <c r="W334" s="12">
@@ -39470,7 +39483,7 @@
       <c r="U335" s="18">
         <v>5</v>
       </c>
-      <c r="V335">
+      <c r="V335" s="10">
         <v>4</v>
       </c>
       <c r="W335" s="12">
@@ -39586,7 +39599,7 @@
       <c r="U336" s="18">
         <v>5</v>
       </c>
-      <c r="V336">
+      <c r="V336" s="10">
         <v>5</v>
       </c>
       <c r="W336" s="12">
@@ -39702,7 +39715,7 @@
       <c r="U337" s="18">
         <v>4</v>
       </c>
-      <c r="V337">
+      <c r="V337" s="10">
         <v>2</v>
       </c>
       <c r="W337" s="12">
@@ -39818,7 +39831,7 @@
       <c r="U338" s="18">
         <v>5</v>
       </c>
-      <c r="V338">
+      <c r="V338" s="10">
         <v>2</v>
       </c>
       <c r="W338" s="12">
@@ -39934,7 +39947,7 @@
       <c r="U339" s="18">
         <v>5</v>
       </c>
-      <c r="V339">
+      <c r="V339" s="10">
         <v>2</v>
       </c>
       <c r="W339" s="12">
@@ -40050,7 +40063,7 @@
       <c r="U340" s="18">
         <v>5</v>
       </c>
-      <c r="V340">
+      <c r="V340" s="10">
         <v>2</v>
       </c>
       <c r="W340" s="12">
@@ -40166,7 +40179,7 @@
       <c r="U341" s="18">
         <v>5</v>
       </c>
-      <c r="V341">
+      <c r="V341" s="10">
         <v>2</v>
       </c>
       <c r="W341" s="12">
@@ -40282,7 +40295,7 @@
       <c r="U342" s="18">
         <v>4</v>
       </c>
-      <c r="V342">
+      <c r="V342" s="10">
         <v>3</v>
       </c>
       <c r="W342" s="12">
@@ -40398,7 +40411,7 @@
       <c r="U343" s="18">
         <v>5</v>
       </c>
-      <c r="V343">
+      <c r="V343" s="10">
         <v>2</v>
       </c>
       <c r="W343" s="12">
@@ -40514,7 +40527,7 @@
       <c r="U344" s="18">
         <v>5</v>
       </c>
-      <c r="V344">
+      <c r="V344" s="10">
         <v>2</v>
       </c>
       <c r="W344" s="12">
@@ -40630,7 +40643,7 @@
       <c r="U345" s="18">
         <v>5</v>
       </c>
-      <c r="V345">
+      <c r="V345" s="10">
         <v>2</v>
       </c>
       <c r="W345" s="12">
@@ -40746,7 +40759,7 @@
       <c r="U346" s="18">
         <v>5</v>
       </c>
-      <c r="V346">
+      <c r="V346" s="10">
         <v>3</v>
       </c>
       <c r="W346" s="12">
@@ -40862,7 +40875,7 @@
       <c r="U347" s="18">
         <v>5</v>
       </c>
-      <c r="V347">
+      <c r="V347" s="10">
         <v>3</v>
       </c>
       <c r="W347" s="12">
@@ -40978,7 +40991,7 @@
       <c r="U348" s="18">
         <v>5</v>
       </c>
-      <c r="V348">
+      <c r="V348" s="10">
         <v>5</v>
       </c>
       <c r="W348" s="12">
@@ -41094,7 +41107,7 @@
       <c r="U349" s="18">
         <v>5</v>
       </c>
-      <c r="V349">
+      <c r="V349" s="10">
         <v>2</v>
       </c>
       <c r="W349" s="12">
@@ -41210,7 +41223,7 @@
       <c r="U350" s="18">
         <v>5</v>
       </c>
-      <c r="V350">
+      <c r="V350" s="10">
         <v>2</v>
       </c>
       <c r="W350" s="12">
@@ -41326,7 +41339,7 @@
       <c r="U351" s="18">
         <v>5</v>
       </c>
-      <c r="V351">
+      <c r="V351" s="10">
         <v>5</v>
       </c>
       <c r="W351" s="12">
@@ -41442,7 +41455,7 @@
       <c r="U352" s="18">
         <v>4</v>
       </c>
-      <c r="V352">
+      <c r="V352" s="10">
         <v>4</v>
       </c>
       <c r="W352" s="12">
@@ -41558,7 +41571,7 @@
       <c r="U353" s="18">
         <v>5</v>
       </c>
-      <c r="V353">
+      <c r="V353" s="10">
         <v>4</v>
       </c>
       <c r="W353" s="12">
@@ -41674,7 +41687,7 @@
       <c r="U354" s="18">
         <v>5</v>
       </c>
-      <c r="V354">
+      <c r="V354" s="10">
         <v>4</v>
       </c>
       <c r="W354" s="12">
@@ -41790,7 +41803,7 @@
       <c r="U355" s="18">
         <v>4</v>
       </c>
-      <c r="V355">
+      <c r="V355" s="10">
         <v>3</v>
       </c>
       <c r="W355" s="12">
@@ -41906,7 +41919,7 @@
       <c r="U356" s="18">
         <v>4</v>
       </c>
-      <c r="V356">
+      <c r="V356" s="10">
         <v>2</v>
       </c>
       <c r="W356" s="12">
@@ -42022,7 +42035,7 @@
       <c r="U357" s="18">
         <v>5</v>
       </c>
-      <c r="V357">
+      <c r="V357" s="10">
         <v>2</v>
       </c>
       <c r="W357" s="12">
@@ -42138,7 +42151,7 @@
       <c r="U358" s="18">
         <v>5</v>
       </c>
-      <c r="V358">
+      <c r="V358" s="10">
         <v>2</v>
       </c>
       <c r="W358" s="12">
@@ -42254,7 +42267,7 @@
       <c r="U359" s="18">
         <v>5</v>
       </c>
-      <c r="V359">
+      <c r="V359" s="10">
         <v>3</v>
       </c>
       <c r="W359" s="12">
@@ -42370,7 +42383,7 @@
       <c r="U360" s="18">
         <v>5</v>
       </c>
-      <c r="V360">
+      <c r="V360" s="10">
         <v>4</v>
       </c>
       <c r="W360" s="12">
@@ -42486,7 +42499,7 @@
       <c r="U361" s="18">
         <v>5</v>
       </c>
-      <c r="V361">
+      <c r="V361" s="10">
         <v>5</v>
       </c>
       <c r="W361" s="12">
@@ -42602,7 +42615,7 @@
       <c r="U362" s="18">
         <v>5</v>
       </c>
-      <c r="V362">
+      <c r="V362" s="10">
         <v>5</v>
       </c>
       <c r="W362" s="12">
@@ -42718,7 +42731,7 @@
       <c r="U363" s="18">
         <v>5</v>
       </c>
-      <c r="V363">
+      <c r="V363" s="10">
         <v>2</v>
       </c>
       <c r="W363" s="12">
@@ -42834,7 +42847,7 @@
       <c r="U364" s="18">
         <v>4</v>
       </c>
-      <c r="V364">
+      <c r="V364" s="10">
         <v>4</v>
       </c>
       <c r="W364" s="12">
@@ -42951,7 +42964,7 @@
       <c r="U365" s="18">
         <v>5</v>
       </c>
-      <c r="V365">
+      <c r="V365" s="10">
         <v>3</v>
       </c>
       <c r="W365" s="12">
@@ -43067,7 +43080,7 @@
       <c r="U366" s="18">
         <v>5</v>
       </c>
-      <c r="V366">
+      <c r="V366" s="10">
         <v>2</v>
       </c>
       <c r="W366" s="12">
@@ -43183,7 +43196,7 @@
       <c r="U367" s="18">
         <v>5</v>
       </c>
-      <c r="V367">
+      <c r="V367" s="10">
         <v>3</v>
       </c>
       <c r="W367" s="12">
@@ -43299,7 +43312,7 @@
       <c r="U368" s="18">
         <v>4</v>
       </c>
-      <c r="V368">
+      <c r="V368" s="10">
         <v>2</v>
       </c>
       <c r="W368" s="12">
@@ -43415,7 +43428,7 @@
       <c r="U369" s="18">
         <v>5</v>
       </c>
-      <c r="V369">
+      <c r="V369" s="10">
         <v>2</v>
       </c>
       <c r="W369" s="12">
@@ -43531,7 +43544,7 @@
       <c r="U370" s="18">
         <v>5</v>
       </c>
-      <c r="V370">
+      <c r="V370" s="10">
         <v>2</v>
       </c>
       <c r="W370" s="12">
@@ -43647,7 +43660,7 @@
       <c r="U371" s="18">
         <v>5</v>
       </c>
-      <c r="V371">
+      <c r="V371" s="10">
         <v>4</v>
       </c>
       <c r="W371" s="12">
@@ -43763,7 +43776,7 @@
       <c r="U372" s="18">
         <v>5</v>
       </c>
-      <c r="V372">
+      <c r="V372" s="10">
         <v>4</v>
       </c>
       <c r="W372" s="12">
@@ -43879,7 +43892,7 @@
       <c r="U373" s="18">
         <v>4</v>
       </c>
-      <c r="V373">
+      <c r="V373" s="10">
         <v>3</v>
       </c>
       <c r="W373" s="12">
@@ -43995,7 +44008,7 @@
       <c r="U374" s="18">
         <v>4</v>
       </c>
-      <c r="V374">
+      <c r="V374" s="10">
         <v>2</v>
       </c>
       <c r="W374" s="12">
@@ -44111,7 +44124,7 @@
       <c r="U375" s="18">
         <v>5</v>
       </c>
-      <c r="V375">
+      <c r="V375" s="10">
         <v>2</v>
       </c>
       <c r="W375" s="12">
@@ -44227,7 +44240,7 @@
       <c r="U376" s="18">
         <v>5</v>
       </c>
-      <c r="V376">
+      <c r="V376" s="10">
         <v>2</v>
       </c>
       <c r="W376" s="12">
@@ -44343,7 +44356,7 @@
       <c r="U377" s="18">
         <v>5</v>
       </c>
-      <c r="V377">
+      <c r="V377" s="10">
         <v>3</v>
       </c>
       <c r="W377" s="12">
@@ -44459,7 +44472,7 @@
       <c r="U378" s="18">
         <v>5</v>
       </c>
-      <c r="V378">
+      <c r="V378" s="10">
         <v>5</v>
       </c>
       <c r="W378" s="12">
@@ -44575,7 +44588,7 @@
       <c r="U379" s="18">
         <v>5</v>
       </c>
-      <c r="V379">
+      <c r="V379" s="10">
         <v>5</v>
       </c>
       <c r="W379" s="12">
@@ -44691,7 +44704,7 @@
       <c r="U380" s="18">
         <v>5</v>
       </c>
-      <c r="V380">
+      <c r="V380" s="10">
         <v>2</v>
       </c>
       <c r="W380" s="12">
@@ -44807,7 +44820,7 @@
       <c r="U381" s="18">
         <v>5</v>
       </c>
-      <c r="V381">
+      <c r="V381" s="10">
         <v>2</v>
       </c>
       <c r="W381" s="12">
@@ -44923,7 +44936,7 @@
       <c r="U382" s="18">
         <v>5</v>
       </c>
-      <c r="V382">
+      <c r="V382" s="10">
         <v>2</v>
       </c>
       <c r="W382" s="12">
@@ -45039,7 +45052,7 @@
       <c r="U383" s="18">
         <v>5</v>
       </c>
-      <c r="V383">
+      <c r="V383" s="10">
         <v>2</v>
       </c>
       <c r="W383" s="12">
@@ -45155,7 +45168,7 @@
       <c r="U384" s="18">
         <v>4</v>
       </c>
-      <c r="V384">
+      <c r="V384" s="10">
         <v>3</v>
       </c>
       <c r="W384" s="12">
@@ -45271,7 +45284,7 @@
       <c r="U385" s="18">
         <v>5</v>
       </c>
-      <c r="V385">
+      <c r="V385" s="10">
         <v>2</v>
       </c>
       <c r="W385" s="12">

</xml_diff>